<commit_message>
ADD: different ways to obtain neighbors
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b25f0c29b1141e6/Uni_Master/Thesis_all/GraphMiner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AB2133F-0047-D449-92DE-D8F09D573630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{1AB2133F-0047-D449-92DE-D8F09D573630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59AAB51D-4095-8B41-9BB2-E836795FF431}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2FD5133B-BC4B-AB4A-AE82-BF3689196BF4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{2FD5133B-BC4B-AB4A-AE82-BF3689196BF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,6 +129,12 @@
       <sz val="14"/>
       <color rgb="FF202124"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -152,10 +158,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -473,7 +480,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,7 +518,7 @@
       <c r="C3">
         <v>23</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>